<commit_message>
Added Keyboard action for login to application
</commit_message>
<xml_diff>
--- a/test-automation-common-sample/src/main/resources/local/excel/TestExcel.xlsx
+++ b/test-automation-common-sample/src/main/resources/local/excel/TestExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kbt7177/Documents/Kaustubh/Automation-Projects/test-automation-common-parent/test-automation-common-sample/src/main/resources/local/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766D40B2-9118-9F4B-B225-58650EAC1E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A097287C-0FE3-EE4C-81A9-2ACAB83BA00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16400" activeTab="1" xr2:uid="{FEB5999E-5E85-6B48-A16A-23B2A654CF4B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Kaustubh</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>springer</t>
+  </si>
+  <si>
+    <t>suvarna</t>
   </si>
 </sst>
 </file>
@@ -417,15 +420,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF97BD7-8515-8144-8327-A07F36517010}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>13539</v>
       </c>
@@ -433,6 +436,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>